<commit_message>
The use-case diagram has been modified. More work-items/ tasks have been assigned and updated.
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Assignment One - ESD\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Assignment One - ESD\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
   <si>
     <t>Backlog - Sprint 1</t>
   </si>
@@ -137,6 +137,24 @@
   </si>
   <si>
     <t>Duration 26/11/18 To 10/12/18</t>
+  </si>
+  <si>
+    <t>Review Use-case diagram.</t>
+  </si>
+  <si>
+    <t>Design three tables; customers, admin, drivers.</t>
+  </si>
+  <si>
+    <t>Create a JSP portal for the admin.</t>
+  </si>
+  <si>
+    <t>Create a JSP portal for the driver.</t>
+  </si>
+  <si>
+    <t>Create a JSP portal for customer.</t>
+  </si>
+  <si>
+    <t>Create login page for all users.</t>
   </si>
 </sst>
 </file>
@@ -1129,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1293,7 +1311,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="45" x14ac:dyDescent="0.25">
@@ -1313,7 +1331,7 @@
         <v>0.2</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1353,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1376,65 +1394,125 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>8</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>1</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="9">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>13</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="11"/>
+      <c r="C24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="10">

</xml_diff>

<commit_message>
I have updated the Usecase, Sprint documentaiton and have started working on the second versio of the class diagram.
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="45">
   <si>
     <t>Backlog - Sprint 1</t>
   </si>
@@ -145,16 +145,22 @@
     <t>Design three tables; customers, admin, drivers.</t>
   </si>
   <si>
-    <t>Create a JSP portal for the admin.</t>
-  </si>
-  <si>
-    <t>Create a JSP portal for the driver.</t>
-  </si>
-  <si>
-    <t>Create a JSP portal for customer.</t>
-  </si>
-  <si>
     <t>Create login page for all users.</t>
+  </si>
+  <si>
+    <t>Signatures:</t>
+  </si>
+  <si>
+    <t>Review class diagram</t>
+  </si>
+  <si>
+    <t>Create a JSP basic portal for the admin.</t>
+  </si>
+  <si>
+    <t>Create a basic JSP portal for the driver.</t>
+  </si>
+  <si>
+    <t>Create a basic JSP portal for customer.</t>
   </si>
 </sst>
 </file>
@@ -330,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -356,12 +362,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="34">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -838,45 +866,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:G26" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="B11:G26"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="27"/>
-    <tableColumn id="2" name="Task:" dataDxfId="26"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="25"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="24"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="23"/>
-    <tableColumn id="6" name="Status:" dataDxfId="22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:H26" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="B11:H26"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="ID:" dataDxfId="28"/>
+    <tableColumn id="2" name="Task:" dataDxfId="27"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="26"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="25"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="24"/>
+    <tableColumn id="6" name="Status:" dataDxfId="23"/>
+    <tableColumn id="7" name="Signatures:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="16"/>
-    <tableColumn id="2" name="Task:" dataDxfId="15"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="14"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="13"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="12"/>
-    <tableColumn id="6" name="Status:" dataDxfId="11"/>
+    <tableColumn id="1" name="ID:" dataDxfId="17"/>
+    <tableColumn id="2" name="Task:" dataDxfId="16"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="15"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="14"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="13"/>
+    <tableColumn id="6" name="Status:" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="5"/>
-    <tableColumn id="2" name="Task:" dataDxfId="4"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="3"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="2"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="1"/>
-    <tableColumn id="6" name="Status:" dataDxfId="0"/>
+    <tableColumn id="1" name="ID:" dataDxfId="6"/>
+    <tableColumn id="2" name="Task:" dataDxfId="5"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="4"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="3"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="2"/>
+    <tableColumn id="6" name="Status:" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1147,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,6 +1188,7 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
@@ -1255,6 +1285,9 @@
       <c r="G11" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
@@ -1275,6 +1308,7 @@
       <c r="G12" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
@@ -1295,6 +1329,7 @@
       <c r="G13" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
@@ -1313,6 +1348,7 @@
       <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
@@ -1333,6 +1369,7 @@
       <c r="G15" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
@@ -1351,10 +1388,11 @@
         <v>2</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>6</v>
       </c>
@@ -1373,8 +1411,9 @@
       <c r="G17" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>7</v>
       </c>
@@ -1393,8 +1432,9 @@
       <c r="G18" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>8</v>
       </c>
@@ -1411,10 +1451,11 @@
         <v>0.1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
@@ -1431,15 +1472,16 @@
         <v>0.2</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>13</v>
@@ -1453,13 +1495,14 @@
       <c r="G21" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>14</v>
@@ -1473,13 +1516,14 @@
       <c r="G22" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>13</v>
@@ -1493,13 +1537,14 @@
       <c r="G23" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>13</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>14</v>
@@ -1513,18 +1558,30 @@
       <c r="G24" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>14</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>15</v>
       </c>
@@ -1533,6 +1590,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created a Gantt Chart
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Assignment One - ESD\Documentation\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ESD Group Assignment\Group11AlphaCab\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="45">
-  <si>
-    <t>Backlog - Sprint 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>Assigned To:</t>
   </si>
@@ -161,6 +158,18 @@
   </si>
   <si>
     <t>Create a basic JSP portal for customer.</t>
+  </si>
+  <si>
+    <t>Status %</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
+  </si>
+  <si>
+    <t>Hours Done:</t>
+  </si>
+  <si>
+    <t>Create Gantt Chart</t>
   </si>
 </sst>
 </file>
@@ -336,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,31 +374,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -704,6 +703,62 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -865,47 +920,1100 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$C$12:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Create a sprint document to record progress.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Create GITHUB Repository.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Incorperate code from Black Board (give to every group) and put it into our repository.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Add the Sprint plan to the GITHUB Repository.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create class diagram (UML)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Create Use-case diagram.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Create a sequence diagram.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Review Use-case diagram.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Design three tables; customers, admin, drivers.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Create a JSP basic portal for the admin.</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Create a basic JSP portal for the driver.</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Create a basic JSP portal for customer.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Create login page for all users.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Review class diagram</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Create Gantt Chart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$F$12:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8C2-4539-A063-FE1B08312B86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$C$12:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Create a sprint document to record progress.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Create GITHUB Repository.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Incorperate code from Black Board (give to every group) and put it into our repository.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Add the Sprint plan to the GITHUB Repository.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create class diagram (UML)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Create Use-case diagram.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Create a sequence diagram.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Review Use-case diagram.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Design three tables; customers, admin, drivers.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Create a JSP basic portal for the admin.</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Create a basic JSP portal for the driver.</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Create a basic JSP portal for customer.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Create login page for all users.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Review class diagram</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Create Gantt Chart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$I$12:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D8C2-4539-A063-FE1B08312B86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="379249672"/>
+        <c:axId val="379256232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="379249672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379256232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="379256232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379249672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74838</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>70758</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>258536</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>13608</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:H26" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <autoFilter ref="B11:H26"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="ID:" dataDxfId="28"/>
-    <tableColumn id="2" name="Task:" dataDxfId="27"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="26"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="25"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="24"/>
-    <tableColumn id="6" name="Status:" dataDxfId="23"/>
-    <tableColumn id="7" name="Signatures:" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:J26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+  <autoFilter ref="B11:J26"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="ID:" dataDxfId="30"/>
+    <tableColumn id="2" name="Task:" dataDxfId="29"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="28"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="27"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="26"/>
+    <tableColumn id="6" name="Status:" dataDxfId="25"/>
+    <tableColumn id="9" name="Status %" dataDxfId="24"/>
+    <tableColumn id="10" name="Hours Done:" dataDxfId="23">
+      <calculatedColumnFormula>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Signatures:" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="17"/>
-    <tableColumn id="2" name="Task:" dataDxfId="16"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="15"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="14"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="13"/>
-    <tableColumn id="6" name="Status:" dataDxfId="12"/>
+    <tableColumn id="1" name="ID:" dataDxfId="16"/>
+    <tableColumn id="2" name="Task:" dataDxfId="15"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="14"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="13"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="12"/>
+    <tableColumn id="6" name="Status:" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="6"/>
-    <tableColumn id="2" name="Task:" dataDxfId="5"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="4"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="3"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="2"/>
-    <tableColumn id="6" name="Status:" dataDxfId="1"/>
+    <tableColumn id="1" name="ID:" dataDxfId="5"/>
+    <tableColumn id="2" name="Task:" dataDxfId="4"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="3"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="2"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="1"/>
+    <tableColumn id="6" name="Status:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1174,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K26"/>
+  <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,140 +2293,153 @@
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="F11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
-        <v>1</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>2</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>
@@ -1327,17 +2448,26 @@
         <v>2</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="2:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>2</v>
+      </c>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
+        <v>3</v>
+      </c>
       <c r="C14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -1346,19 +2476,26 @@
         <v>6</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>6</v>
+      </c>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>4</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="9">
         <v>1</v>
@@ -1367,19 +2504,26 @@
         <v>0.2</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>5</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -1388,19 +2532,26 @@
         <v>2</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H16" s="16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
@@ -1409,19 +2560,26 @@
         <v>1</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H17" s="16">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="9">
         <v>1</v>
@@ -1432,17 +2590,24 @@
       <c r="G18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="9">
         <v>1</v>
@@ -1451,19 +2616,26 @@
         <v>0.1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H19" s="16">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
@@ -1472,19 +2644,26 @@
         <v>0.2</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H20" s="16">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="9">
         <v>1</v>
@@ -1493,19 +2672,26 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="I21" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>
@@ -1514,19 +2700,26 @@
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="I22" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -1535,19 +2728,26 @@
         <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="I23" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>13</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" s="9">
         <v>1</v>
@@ -1558,45 +2758,77 @@
       <c r="G24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="16">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>14</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="9">
         <v>1</v>
       </c>
       <c r="F25" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H25" s="16">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>3</v>
+      </c>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>15</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="13">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="18">
+        <v>1</v>
+      </c>
+      <c r="I26" s="13">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1623,95 +2855,95 @@
   <sheetData>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1893,95 +3125,95 @@
   <sheetData>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Amend planning documentation to accomodate additional requirements
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ESD Group Assignment\Group11AlphaCab\Documentation\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ESDProject1\Group11AlphaCab\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>Assigned To:</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Review Use-case diagram.</t>
   </si>
   <si>
-    <t>Design three tables; customers, admin, drivers.</t>
-  </si>
-  <si>
     <t>Create login page for all users.</t>
   </si>
   <si>
@@ -170,6 +167,18 @@
   </si>
   <si>
     <t>Create Gantt Chart</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Design three tables; customers, users and drivers.</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -340,12 +349,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,12 +405,77 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="39">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -956,9 +1043,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$12:$C$26</c:f>
+              <c:f>'Sprint 1'!$C$12:$C$23</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Create a sprint document to record progress.</c:v>
                 </c:pt>
@@ -984,24 +1071,15 @@
                   <c:v>Review Use-case diagram.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Design three tables; customers, admin, drivers.</c:v>
+                  <c:v>Design three tables; customers, users and drivers.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Create a JSP basic portal for the admin.</c:v>
+                  <c:v>Create login page for all users.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Create a basic JSP portal for the driver.</c:v>
+                  <c:v>Review class diagram</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Create a basic JSP portal for customer.</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Create login page for all users.</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Review class diagram</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>Create Gantt Chart</c:v>
                 </c:pt>
               </c:strCache>
@@ -1009,10 +1087,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$F$12:$F$26</c:f>
+              <c:f>'Sprint 1'!$F$12:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1044,18 +1122,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1082,9 +1151,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$12:$C$26</c:f>
+              <c:f>'Sprint 1'!$C$12:$C$23</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Create a sprint document to record progress.</c:v>
                 </c:pt>
@@ -1110,24 +1179,15 @@
                   <c:v>Review Use-case diagram.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Design three tables; customers, admin, drivers.</c:v>
+                  <c:v>Design three tables; customers, users and drivers.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Create a JSP basic portal for the admin.</c:v>
+                  <c:v>Create login page for all users.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Create a basic JSP portal for the driver.</c:v>
+                  <c:v>Review class diagram</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Create a basic JSP portal for customer.</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Create login page for all users.</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Review class diagram</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>Create Gantt Chart</c:v>
                 </c:pt>
               </c:strCache>
@@ -1135,10 +1195,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$I$12:$I$26</c:f>
+              <c:f>'Sprint 1'!$I$12:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1158,7 +1218,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.1</c:v>
@@ -1167,21 +1227,12 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1970,50 +2021,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:J26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
-  <autoFilter ref="B11:J26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:J23" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B11:J23"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="ID:" dataDxfId="30"/>
-    <tableColumn id="2" name="Task:" dataDxfId="29"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="28"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="27"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="26"/>
-    <tableColumn id="6" name="Status:" dataDxfId="25"/>
-    <tableColumn id="9" name="Status %" dataDxfId="24"/>
-    <tableColumn id="10" name="Hours Done:" dataDxfId="23">
+    <tableColumn id="1" name="ID:" dataDxfId="33"/>
+    <tableColumn id="2" name="Task:" dataDxfId="32"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="31"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="30"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="29"/>
+    <tableColumn id="6" name="Status:" dataDxfId="28"/>
+    <tableColumn id="9" name="Status %" dataDxfId="27"/>
+    <tableColumn id="10" name="Hours Done:" dataDxfId="26">
       <calculatedColumnFormula>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Signatures:" dataDxfId="22"/>
+    <tableColumn id="7" name="Signatures:" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="B11:G26"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="16"/>
-    <tableColumn id="2" name="Task:" dataDxfId="15"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="14"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="13"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="12"/>
-    <tableColumn id="6" name="Status:" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:J26" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B11:J26"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="ID:" dataDxfId="19"/>
+    <tableColumn id="2" name="Task:" dataDxfId="18"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="17"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="16"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="15"/>
+    <tableColumn id="6" name="Status:" dataDxfId="14"/>
+    <tableColumn id="7" name="Column1" dataDxfId="2"/>
+    <tableColumn id="8" name="Column2" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Column3" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="5"/>
-    <tableColumn id="2" name="Task:" dataDxfId="4"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="3"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="2"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="1"/>
-    <tableColumn id="6" name="Status:" dataDxfId="0"/>
+    <tableColumn id="1" name="ID:" dataDxfId="8"/>
+    <tableColumn id="2" name="Task:" dataDxfId="7"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="6"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="5"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="4"/>
+    <tableColumn id="6" name="Status:" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2282,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L26"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,7 +2359,7 @@
   <sheetData>
     <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -2394,13 +2450,13 @@
         <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
@@ -2588,14 +2644,14 @@
         <v>2</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I18" s="9">
         <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="9"/>
     </row>
@@ -2632,7 +2688,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>13</v>
@@ -2660,10 +2716,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="9">
         <v>1</v>
@@ -2672,156 +2728,72 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H21" s="16">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="9">
         <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>
       </c>
       <c r="F22" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H22" s="16">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="9">
         <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>12</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="9">
-        <v>1</v>
-      </c>
-      <c r="F23" s="9">
-        <v>1</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="I23" s="9">
+      <c r="C23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13">
+        <v>1</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="18">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13">
         <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
-      </c>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
-        <v>13</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="9">
-        <v>1</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="16">
-        <v>1</v>
-      </c>
-      <c r="I24" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="10">
-        <v>14</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="9">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9">
-        <v>3</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="16">
-        <v>1</v>
-      </c>
-      <c r="I25" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>3</v>
-      </c>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>15</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="13">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13">
-        <v>1</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="18">
-        <v>1</v>
-      </c>
-      <c r="I26" s="13">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J26" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2838,7 +2810,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,34 +2917,99 @@
       <c r="G11" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="15">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>2</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="11"/>
+      <c r="C13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>2</v>
+      </c>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>6</v>
+      </c>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
@@ -2983,6 +3020,12 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
@@ -2993,8 +3036,14 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="9"/>
+      <c r="I16" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>6</v>
       </c>
@@ -3003,8 +3052,14 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="9"/>
+      <c r="I17" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>7</v>
       </c>
@@ -3013,8 +3068,14 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>2</v>
+      </c>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>8</v>
       </c>
@@ -3023,8 +3084,14 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
@@ -3033,8 +3100,14 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="9"/>
+      <c r="I20" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
@@ -3043,8 +3116,14 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="9"/>
+      <c r="I21" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
@@ -3053,8 +3132,14 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>3</v>
+      </c>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
@@ -3063,8 +3148,14 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="9"/>
+      <c r="I23" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>13</v>
       </c>
@@ -3073,8 +3164,14 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9" t="e">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>14</v>
       </c>
@@ -3083,8 +3180,14 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="9"/>
+      <c r="I25" s="9" t="e">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>15</v>
       </c>
@@ -3093,6 +3196,12 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13" t="e">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create sprint plan 2 with a new Gantt chart.
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ESD Group Assignment\Group11AlphaCab\Documentation\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Assignment One - ESD\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="61">
   <si>
     <t>Assigned To:</t>
   </si>
@@ -151,15 +151,6 @@
     <t>Review class diagram</t>
   </si>
   <si>
-    <t>Create a JSP basic portal for the admin.</t>
-  </si>
-  <si>
-    <t>Create a basic JSP portal for the driver.</t>
-  </si>
-  <si>
-    <t>Create a basic JSP portal for customer.</t>
-  </si>
-  <si>
     <t>Status %</t>
   </si>
   <si>
@@ -170,13 +161,61 @@
   </si>
   <si>
     <t>Create Gantt Chart</t>
+  </si>
+  <si>
+    <t>Start date:</t>
+  </si>
+  <si>
+    <t>End Date:</t>
+  </si>
+  <si>
+    <t>Create portal for users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Estimated Days:</t>
+  </si>
+  <si>
+    <t>Allow admin to view bookings.</t>
+  </si>
+  <si>
+    <t>Create version 3 of the class diagram.</t>
+  </si>
+  <si>
+    <t>Create a Booking table.</t>
+  </si>
+  <si>
+    <t>14/11/018</t>
+  </si>
+  <si>
+    <t>Create Sprint two tasks.</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>Create customer from bookings.</t>
+  </si>
+  <si>
+    <t>Allow drivers to see bookings</t>
+  </si>
+  <si>
+    <t>Assign Driver to customer.</t>
+  </si>
+  <si>
+    <t>Allow a customer to book a taxi.</t>
+  </si>
+  <si>
+    <t>Allow admin to create invoices.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +233,13 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -340,12 +386,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,12 +443,179 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="43">
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -939,14 +1166,150 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start date:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$C$12:$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Create a sprint document to record progress.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Create GITHUB Repository.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Incorperate code from Black Board (give to every group) and put it into our repository.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Add the Sprint plan to the GITHUB Repository.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create class diagram (UML)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Create Use-case diagram.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Create a sequence diagram.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Review Use-case diagram.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Design three tables; customers, admin, drivers.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Create portal for users.</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Create login page for all users.</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Review class diagram</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Create Gantt Chart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$F$12:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43409</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7576-42AB-BCBA-5745B1B13A6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$H$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Days:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -956,9 +1319,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$12:$C$26</c:f>
+              <c:f>'Sprint 1'!$C$12:$C$24</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Create a sprint document to record progress.</c:v>
                 </c:pt>
@@ -987,21 +1350,15 @@
                   <c:v>Design three tables; customers, admin, drivers.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Create a JSP basic portal for the admin.</c:v>
+                  <c:v>Create portal for users.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Create a basic JSP portal for the driver.</c:v>
+                  <c:v>Create login page for all users.</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Create a basic JSP portal for customer.</c:v>
+                  <c:v>Review class diagram</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Create login page for all users.</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Review class diagram</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>Create Gantt Chart</c:v>
                 </c:pt>
               </c:strCache>
@@ -1009,36 +1366,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$F$12:$F$26</c:f>
+              <c:f>'Sprint 1'!$H$12:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1050,12 +1407,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1063,133 +1414,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D8C2-4539-A063-FE1B08312B86}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sprint 1'!$C$12:$C$26</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Create a sprint document to record progress.</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Create GITHUB Repository.</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Incorperate code from Black Board (give to every group) and put it into our repository.</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Add the Sprint plan to the GITHUB Repository.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Create class diagram (UML)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Create Use-case diagram.</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Create a sequence diagram.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Review Use-case diagram.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Design three tables; customers, admin, drivers.</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Create a JSP basic portal for the admin.</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Create a basic JSP portal for the driver.</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Create a basic JSP portal for customer.</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Create login page for all users.</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Review class diagram</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Create Gantt Chart</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 1'!$I$12:$I$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D8C2-4539-A063-FE1B08312B86}"/>
+              <c16:uniqueId val="{00000004-7576-42AB-BCBA-5745B1B13A6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1201,14 +1426,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="379249672"/>
-        <c:axId val="379256232"/>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="366856632"/>
+        <c:axId val="366860896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="379249672"/>
+        <c:axId val="366856632"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1234,7 +1460,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1249,7 +1475,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379256232"/>
+        <c:crossAx val="366860896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1257,12 +1483,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379256232"/>
+        <c:axId val="366860896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1277,7 +1503,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1308,7 +1534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379249672"/>
+        <c:crossAx val="366856632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1320,10 +1546,386 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
-      <c:overlay val="0"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start date:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$12:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Allow a customer to book a taxi.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Allow admin to view bookings.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Create version 3 of the class diagram.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Create a Booking table.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create Sprint two tasks.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Create customer from bookings.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Allow drivers to see bookings</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Assign Driver to customer.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Allow admin to create invoices.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$F$12:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43418</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43417</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D278-4319-A5C9-A4A980E07EF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$H$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Days:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$12:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Allow a customer to book a taxi.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Allow admin to view bookings.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Create version 3 of the class diagram.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Create a Booking table.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create Sprint two tasks.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Create customer from bookings.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Allow drivers to see bookings</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Assign Driver to customer.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Allow admin to create invoices.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$H$12:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D278-4319-A5C9-A4A980E07EF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="146"/>
+        <c:overlap val="100"/>
+        <c:axId val="600576512"/>
+        <c:axId val="600583072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="600576512"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="600583072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="600583072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="dd/mm" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="600576512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1331,27 +1933,7 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1429,8 +2011,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1934,24 +2556,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>74838</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>70758</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>13606</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>258536</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1970,50 +3132,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:J26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
-  <autoFilter ref="B11:J26"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="ID:" dataDxfId="30"/>
-    <tableColumn id="2" name="Task:" dataDxfId="29"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="28"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="27"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="26"/>
-    <tableColumn id="6" name="Status:" dataDxfId="25"/>
-    <tableColumn id="9" name="Status %" dataDxfId="24"/>
-    <tableColumn id="10" name="Hours Done:" dataDxfId="23">
-      <calculatedColumnFormula>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:L24" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+  <autoFilter ref="B11:L24"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="ID:" dataDxfId="37"/>
+    <tableColumn id="2" name="Task:" dataDxfId="36"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="35"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="34"/>
+    <tableColumn id="8" name="Start date:" dataDxfId="5">
+      <calculatedColumnFormula>DATE(2018,10,29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Signatures:" dataDxfId="22"/>
+    <tableColumn id="11" name="End Date:" dataDxfId="6"/>
+    <tableColumn id="5" name="Estimated Days:" dataDxfId="33"/>
+    <tableColumn id="6" name="Status:" dataDxfId="32"/>
+    <tableColumn id="9" name="Status %" dataDxfId="31"/>
+    <tableColumn id="10" name="Hours Done:" dataDxfId="30">
+      <calculatedColumnFormula>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Signatures:" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="B11:G26"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="16"/>
-    <tableColumn id="2" name="Task:" dataDxfId="15"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="14"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="13"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="12"/>
-    <tableColumn id="6" name="Status:" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:L26" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="B11:L26"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="ID:" dataDxfId="23"/>
+    <tableColumn id="2" name="Task:" dataDxfId="22"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="21"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="20"/>
+    <tableColumn id="5" name="Start date:" dataDxfId="19"/>
+    <tableColumn id="6" name="End Date:" dataDxfId="18"/>
+    <tableColumn id="7" name="Estimated Days:" dataDxfId="4"/>
+    <tableColumn id="8" name="Status:" dataDxfId="3"/>
+    <tableColumn id="9" name="Status %" dataDxfId="2"/>
+    <tableColumn id="10" name="Hours Done:" dataDxfId="0"/>
+    <tableColumn id="11" name="Signatures:" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="5"/>
-    <tableColumn id="2" name="Task:" dataDxfId="4"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="3"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="2"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="1"/>
-    <tableColumn id="6" name="Status:" dataDxfId="0"/>
+    <tableColumn id="1" name="ID:" dataDxfId="12"/>
+    <tableColumn id="2" name="Task:" dataDxfId="11"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="10"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="9"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="8"/>
+    <tableColumn id="6" name="Status:" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2282,10 +3453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L26"/>
+  <dimension ref="B2:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,14 +3467,15 @@
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="10" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -2374,7 +3546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>1</v>
       </c>
@@ -2387,19 +3559,25 @@
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2416,20 +3594,27 @@
       <c r="E12" s="9">
         <v>1</v>
       </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="F12" s="19">
+        <f t="shared" ref="F12" si="0">DATE(2018,10,29)</f>
+        <v>43402</v>
+      </c>
+      <c r="G12" s="19">
+        <v>43402</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="17">
-        <v>1</v>
-      </c>
-      <c r="I12" s="15">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="15"/>
+      <c r="J12" s="17">
+        <v>1</v>
+      </c>
+      <c r="K12" s="15">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="15"/>
     </row>
     <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
@@ -2444,20 +3629,27 @@
       <c r="E13" s="9">
         <v>1</v>
       </c>
-      <c r="F13" s="9">
-        <v>2</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="19">
+        <f>DATE(2018,10,29)</f>
+        <v>43402</v>
+      </c>
+      <c r="G13" s="19">
+        <v>43402</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="16">
-        <v>1</v>
-      </c>
-      <c r="I13" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>2</v>
-      </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="16">
+        <v>1</v>
+      </c>
+      <c r="K13" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
@@ -2472,20 +3664,26 @@
       <c r="E14" s="9">
         <v>1</v>
       </c>
-      <c r="F14" s="9">
-        <v>6</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="F14" s="19">
+        <v>43403</v>
+      </c>
+      <c r="G14" s="19">
+        <v>43403</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="16">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>6</v>
-      </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="16">
+        <v>1</v>
+      </c>
+      <c r="K14" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
@@ -2500,20 +3698,26 @@
       <c r="E15" s="9">
         <v>1</v>
       </c>
-      <c r="F15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="19">
+        <v>43402</v>
+      </c>
+      <c r="G15" s="19">
+        <v>43402</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="16">
-        <v>1</v>
-      </c>
-      <c r="I15" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
-      </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="16">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
@@ -2528,22 +3732,28 @@
       <c r="E16" s="9">
         <v>1</v>
       </c>
-      <c r="F16" s="9">
-        <v>2</v>
-      </c>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="19">
+        <v>43405</v>
+      </c>
+      <c r="G16" s="19">
+        <v>43405</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>2</v>
-      </c>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J16" s="16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>6</v>
       </c>
@@ -2556,22 +3766,28 @@
       <c r="E17" s="9">
         <v>1</v>
       </c>
-      <c r="F17" s="9">
-        <v>1</v>
-      </c>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="19">
+        <v>43405</v>
+      </c>
+      <c r="G17" s="19">
+        <v>43405</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="16">
-        <v>1</v>
-      </c>
-      <c r="I17" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J17" s="16">
+        <v>1</v>
+      </c>
+      <c r="K17" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>7</v>
       </c>
@@ -2584,22 +3800,28 @@
       <c r="E18" s="9">
         <v>1</v>
       </c>
-      <c r="F18" s="9">
-        <v>2</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I18" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="F18" s="19">
+        <v>43405</v>
+      </c>
+      <c r="G18" s="19">
+        <v>43405</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="16">
+        <v>1</v>
+      </c>
+      <c r="K18" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>8</v>
       </c>
@@ -2612,22 +3834,28 @@
       <c r="E19" s="9">
         <v>1</v>
       </c>
-      <c r="F19" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="19">
+        <v>43405</v>
+      </c>
+      <c r="G19" s="19">
+        <v>43405</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="16">
-        <v>1</v>
-      </c>
-      <c r="I19" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.1</v>
-      </c>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J19" s="16">
+        <v>1</v>
+      </c>
+      <c r="K19" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="2:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
@@ -2640,55 +3868,67 @@
       <c r="E20" s="9">
         <v>1</v>
       </c>
-      <c r="F20" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G20" s="11" t="s">
+      <c r="F20" s="19">
+        <v>43409</v>
+      </c>
+      <c r="G20" s="19">
+        <v>43409</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="16">
-        <v>1</v>
-      </c>
-      <c r="I20" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
-      </c>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J20" s="16">
+        <v>1</v>
+      </c>
+      <c r="K20" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E21" s="9">
         <v>1</v>
       </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="I21" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
-      </c>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="19">
+        <v>43410</v>
+      </c>
+      <c r="G21" s="19">
+        <v>43410</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="16">
+        <v>1</v>
+      </c>
+      <c r="K21" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>13</v>
@@ -2696,27 +3936,33 @@
       <c r="E22" s="9">
         <v>1</v>
       </c>
-      <c r="F22" s="9">
-        <v>1</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="I22" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
-      </c>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="F22" s="19">
+        <v>43410</v>
+      </c>
+      <c r="G22" s="19">
+        <v>43410</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="16">
+        <v>1</v>
+      </c>
+      <c r="K22" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>12</v>
@@ -2724,108 +3970,72 @@
       <c r="E23" s="9">
         <v>1</v>
       </c>
-      <c r="F23" s="9">
-        <v>1</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="I23" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>0.2</v>
-      </c>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
+      <c r="F23" s="19">
+        <v>43405</v>
+      </c>
+      <c r="G23" s="19">
+        <v>43405</v>
+      </c>
+      <c r="H23" s="9">
+        <v>1</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="16">
+        <v>1</v>
+      </c>
+      <c r="K23" s="9">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>13</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="9">
-        <v>1</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="C24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="13">
+        <v>1</v>
+      </c>
+      <c r="F24" s="19">
+        <v>43415</v>
+      </c>
+      <c r="G24" s="19">
+        <v>43415</v>
+      </c>
+      <c r="H24" s="13">
+        <v>1</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="16">
-        <v>1</v>
-      </c>
-      <c r="I24" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="10">
-        <v>14</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="9">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9">
-        <v>3</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="16">
-        <v>1</v>
-      </c>
-      <c r="I25" s="9">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>3</v>
-      </c>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>15</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="13">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13">
-        <v>1</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="18">
-        <v>1</v>
-      </c>
-      <c r="I26" s="13">
-        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Hours:]])</f>
-        <v>1</v>
-      </c>
-      <c r="J26" s="13"/>
+      <c r="J24" s="18">
+        <v>1</v>
+      </c>
+      <c r="K24" s="13">
+        <f>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AF29" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F14:F16 F17:G17 F18:F24" calculatedColumn="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -2835,10 +4045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K26"/>
+  <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,23 +4059,25 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
@@ -2882,7 +4094,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
@@ -2899,7 +4111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
@@ -2910,7 +4122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
@@ -2921,12 +4133,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>1</v>
       </c>
@@ -2939,166 +4151,433 @@
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="19">
+        <v>43416</v>
+      </c>
+      <c r="G12" s="19">
+        <v>43416</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>2</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19">
+        <v>43417</v>
+      </c>
+      <c r="G13" s="19">
+        <v>43417</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="20">
+        <v>0</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="19">
+        <v>43418</v>
+      </c>
+      <c r="G14" s="19">
+        <v>43418</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="20">
+        <v>0</v>
+      </c>
+      <c r="K14" s="25">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>4</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="19">
+        <v>43418</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="20">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25">
+        <v>0</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>5</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="19">
+        <v>43416</v>
+      </c>
+      <c r="G16" s="19">
+        <v>43416</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="25">
+        <v>1</v>
+      </c>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>6</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="19">
+        <v>43417</v>
+      </c>
+      <c r="G17" s="19">
+        <v>43418</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0</v>
+      </c>
+      <c r="K17" s="25">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>7</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="19">
+        <v>43419</v>
+      </c>
+      <c r="G18" s="19">
+        <v>43419</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="20">
+        <v>0</v>
+      </c>
+      <c r="K18" s="25">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>8</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="19">
+        <v>43419</v>
+      </c>
+      <c r="G19" s="19">
+        <v>43419</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="20">
+        <v>0</v>
+      </c>
+      <c r="K19" s="25">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="19">
+        <v>43424</v>
+      </c>
+      <c r="G20" s="19">
+        <v>43424</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="25">
+        <v>0</v>
+      </c>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>11</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
+      <c r="E23" s="9">
+        <v>1</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>13</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13">
+        <v>1</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>14</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>15</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="13">
+        <v>1</v>
+      </c>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated the sprint plan.
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Assignment One - ESD\Documentation\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Group11AlphaCab\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
   <si>
     <t>Assigned To:</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Allow admin to create invoices.</t>
+  </si>
+  <si>
+    <t>Redesign tables to appear modern</t>
   </si>
 </sst>
 </file>
@@ -473,150 +476,6 @@
   </cellStyles>
   <dxfs count="43">
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -776,6 +635,102 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1014,6 +969,54 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1630,7 +1633,7 @@
             <c:strRef>
               <c:f>'Sprint 2'!$C$12:$C$26</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Allow a customer to book a taxi.</c:v>
                 </c:pt>
@@ -1657,6 +1660,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Allow admin to create invoices.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Redesign tables to appear modern</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1693,6 +1699,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>43424</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,7 +1742,7 @@
             <c:strRef>
               <c:f>'Sprint 2'!$C$12:$C$26</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Allow a customer to book a taxi.</c:v>
                 </c:pt>
@@ -1760,6 +1769,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Allow admin to create invoices.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Redesign tables to appear modern</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1795,6 +1807,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3139,52 +3154,52 @@
     <tableColumn id="2" name="Task:" dataDxfId="36"/>
     <tableColumn id="3" name="Assigned To:" dataDxfId="35"/>
     <tableColumn id="4" name="Effort Points:" dataDxfId="34"/>
-    <tableColumn id="8" name="Start date:" dataDxfId="5">
+    <tableColumn id="8" name="Start date:" dataDxfId="33">
       <calculatedColumnFormula>DATE(2018,10,29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="End Date:" dataDxfId="6"/>
-    <tableColumn id="5" name="Estimated Days:" dataDxfId="33"/>
-    <tableColumn id="6" name="Status:" dataDxfId="32"/>
-    <tableColumn id="9" name="Status %" dataDxfId="31"/>
-    <tableColumn id="10" name="Hours Done:" dataDxfId="30">
+    <tableColumn id="11" name="End Date:" dataDxfId="32"/>
+    <tableColumn id="5" name="Estimated Days:" dataDxfId="31"/>
+    <tableColumn id="6" name="Status:" dataDxfId="30"/>
+    <tableColumn id="9" name="Status %" dataDxfId="29"/>
+    <tableColumn id="10" name="Hours Done:" dataDxfId="28">
       <calculatedColumnFormula>SUM(Table3[[#This Row],[Status %]]  * Table3[[#This Row],[Estimated Days:]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Signatures:" dataDxfId="29"/>
+    <tableColumn id="7" name="Signatures:" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:L26" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:L26" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B11:L26"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID:" dataDxfId="23"/>
-    <tableColumn id="2" name="Task:" dataDxfId="22"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="21"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="20"/>
-    <tableColumn id="5" name="Start date:" dataDxfId="19"/>
-    <tableColumn id="6" name="End Date:" dataDxfId="18"/>
-    <tableColumn id="7" name="Estimated Days:" dataDxfId="4"/>
-    <tableColumn id="8" name="Status:" dataDxfId="3"/>
-    <tableColumn id="9" name="Status %" dataDxfId="2"/>
-    <tableColumn id="10" name="Hours Done:" dataDxfId="0"/>
-    <tableColumn id="11" name="Signatures:" dataDxfId="1"/>
+    <tableColumn id="1" name="ID:" dataDxfId="21"/>
+    <tableColumn id="2" name="Task:" dataDxfId="20"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="19"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="18"/>
+    <tableColumn id="5" name="Start date:" dataDxfId="17"/>
+    <tableColumn id="6" name="End Date:" dataDxfId="16"/>
+    <tableColumn id="7" name="Estimated Days:" dataDxfId="15"/>
+    <tableColumn id="8" name="Status:" dataDxfId="14"/>
+    <tableColumn id="9" name="Status %" dataDxfId="13"/>
+    <tableColumn id="10" name="Hours Done:" dataDxfId="12"/>
+    <tableColumn id="11" name="Signatures:" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="12"/>
-    <tableColumn id="2" name="Task:" dataDxfId="11"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="10"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="9"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="8"/>
-    <tableColumn id="6" name="Status:" dataDxfId="7"/>
+    <tableColumn id="1" name="ID:" dataDxfId="5"/>
+    <tableColumn id="2" name="Task:" dataDxfId="4"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="3"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="2"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="1"/>
+    <tableColumn id="6" name="Status:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4048,7 +4063,7 @@
   <dimension ref="B2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4199,10 +4214,10 @@
         <v>8</v>
       </c>
       <c r="J12" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="15"/>
     </row>
@@ -4232,10 +4247,10 @@
         <v>8</v>
       </c>
       <c r="J13" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="9"/>
     </row>
@@ -4298,10 +4313,10 @@
         <v>8</v>
       </c>
       <c r="J15" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="9"/>
     </row>
@@ -4331,7 +4346,7 @@
         <v>55</v>
       </c>
       <c r="J16" s="20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K16" s="25">
         <v>1</v>
@@ -4470,21 +4485,37 @@
       </c>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>10</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="9">
         <v>1</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="25"/>
+      <c r="F21" s="19">
+        <v>43416</v>
+      </c>
+      <c r="G21" s="19">
+        <v>43416</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="20">
+        <v>1</v>
+      </c>
+      <c r="K21" s="25">
+        <v>1</v>
+      </c>
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edited the tdf for and Gantt chart
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nstu-nas01.uwe.ac.uk\users1$\c2-sellick\Windows\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ESD Group Assignment\Group11AlphaCab\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="66">
   <si>
     <t>Assigned To:</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Create the TDF.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogdan-Stefan Pop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Gantt chart </t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -485,6 +491,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1651,21 +1660,45 @@
             <c:strRef>
               <c:f>'Sprint 2'!$C$12:$C$28</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Allow a customer to book a taxi.</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Allow admin to view bookings.</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>Create version 3 of the class diagram.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Create a Booking table.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create Sprint two tasks.</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Create customer from bookings.</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>Allow drivers to see bookings</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>Assign Driver to customer.</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>Allow admin to create invoices.</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Redesign tables to appear modern</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Create new versions of the sequence diagrams</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Create the TDF.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Update Gantt chart </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1675,21 +1708,45 @@
               <c:f>'Sprint 2'!$F$12:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>43417</c:v>
+                  <c:v>43416</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>43417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43419</c:v>
+                  <c:v>43418</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43419</c:v>
+                  <c:v>43418</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43417</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43424</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43427</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43427</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1730,21 +1787,45 @@
             <c:strRef>
               <c:f>'Sprint 2'!$C$12:$C$28</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Allow a customer to book a taxi.</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Allow admin to view bookings.</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>Create version 3 of the class diagram.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Create a Booking table.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Create Sprint two tasks.</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Create customer from bookings.</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>Allow drivers to see bookings</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>Assign Driver to customer.</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>Allow admin to create invoices.</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Redesign tables to appear modern</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Create new versions of the sequence diagrams</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Create the TDF.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Update Gantt chart </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1754,12 +1835,12 @@
               <c:f>'Sprint 2'!$H$12:$H$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1768,6 +1849,30 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3073,16 +3178,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>190498</xdr:rowOff>
+      <xdr:rowOff>180973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3130,13 +3235,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:L28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="B11:L28">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Kieran Bourne"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B11:L28"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID:" dataDxfId="21"/>
     <tableColumn id="2" name="Task:" dataDxfId="20"/>
@@ -4026,15 +4125,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
@@ -4152,7 +4251,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>1</v>
       </c>
@@ -4218,7 +4317,7 @@
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="2:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>3</v>
       </c>
@@ -4251,7 +4350,7 @@
       </c>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="2:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>4</v>
       </c>
@@ -4267,7 +4366,7 @@
       <c r="F15" s="19">
         <v>43418</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="31" t="s">
         <v>53</v>
       </c>
       <c r="H15" s="9">
@@ -4284,7 +4383,7 @@
       </c>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="2:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>5</v>
       </c>
@@ -4406,17 +4505,17 @@
         <v>1</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="25">
         <v>0</v>
       </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="2:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>9</v>
       </c>
@@ -4482,7 +4581,7 @@
       </c>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="2:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>11</v>
       </c>
@@ -4515,7 +4614,7 @@
       </c>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="2:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>12</v>
       </c>
@@ -4523,7 +4622,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -4548,20 +4647,38 @@
       </c>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="20"/>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>13</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="13">
+        <v>1</v>
+      </c>
+      <c r="F24" s="19">
+        <v>43427</v>
+      </c>
+      <c r="G24" s="19">
+        <v>43427</v>
+      </c>
+      <c r="H24" s="9">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="20">
+        <v>1</v>
+      </c>
       <c r="K24" s="25"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -4574,7 +4691,7 @@
       <c r="K25" s="25"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -4587,7 +4704,7 @@
       <c r="K26" s="26"/>
       <c r="L26" s="13"/>
     </row>
-    <row r="27" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -4600,7 +4717,7 @@
       <c r="K27" s="20"/>
       <c r="L27" s="13"/>
     </row>
-    <row r="28" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>

</xml_diff>

<commit_message>
Updated tdf and sprint plans.
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -193,9 +193,6 @@
     <t>Create Sprint two tasks.</t>
   </si>
   <si>
-    <t>Create customer from bookings.</t>
-  </si>
-  <si>
     <t>Allow drivers to see bookings</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">Update Gantt chart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevent non users from creating bookings. </t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1677,7 @@
                   <c:v>Create Sprint two tasks.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Create customer from bookings.</c:v>
+                  <c:v>Prevent non users from creating bookings. </c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Allow drivers to see bookings</c:v>
@@ -1804,7 +1804,7 @@
                   <c:v>Create Sprint two tasks.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Create customer from bookings.</c:v>
+                  <c:v>Prevent non users from creating bookings. </c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Allow drivers to see bookings</c:v>
@@ -4125,8 +4125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4256,7 +4256,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>12</v>
@@ -4280,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="15"/>
     </row>
@@ -4325,7 +4325,7 @@
         <v>51</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -4340,13 +4340,13 @@
         <v>1</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J14" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="9"/>
     </row>
@@ -4416,12 +4416,12 @@
       </c>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>13</v>
@@ -4439,13 +4439,13 @@
         <v>2</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J17" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="9"/>
     </row>
@@ -4454,7 +4454,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>13</v>
@@ -4472,10 +4472,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J18" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="25">
         <v>1</v>
@@ -4487,7 +4487,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>12</v>
@@ -4520,7 +4520,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>12</v>
@@ -4538,13 +4538,13 @@
         <v>1</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J20" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="9"/>
     </row>
@@ -4553,7 +4553,7 @@
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>13</v>
@@ -4586,7 +4586,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>16</v>
@@ -4604,13 +4604,13 @@
         <v>1</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J22" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="9"/>
     </row>
@@ -4619,10 +4619,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -4637,13 +4637,13 @@
         <v>1</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J23" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="9"/>
     </row>
@@ -4652,7 +4652,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>15</v>
@@ -4675,7 +4675,9 @@
       <c r="J24" s="20">
         <v>1</v>
       </c>
-      <c r="K24" s="25"/>
+      <c r="K24" s="25">
+        <v>1</v>
+      </c>
       <c r="L24" s="9"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added the required tasks to the Gantt Chart
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Sprint Plans.xlsx
+++ b/Documentation/Planning/Sprint Plans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nstu-nas01.uwe.ac.uk\users1$\c2-sellick\Windows\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ESD Group Assignment\Group11AlphaCab\Documentation\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="77">
   <si>
     <t>Assigned To:</t>
   </si>
@@ -224,6 +224,39 @@
   </si>
   <si>
     <t>Create the Google Map Servlet</t>
+  </si>
+  <si>
+    <t>Bogdan Pop</t>
+  </si>
+  <si>
+    <t>Test Cases (1-5)</t>
+  </si>
+  <si>
+    <t>Test Cases (6-10)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Adding reporting functionality</t>
+  </si>
+  <si>
+    <t>Refactoring code</t>
+  </si>
+  <si>
+    <t>Display customer served per day</t>
+  </si>
+  <si>
+    <t>Create a daily report</t>
+  </si>
+  <si>
+    <t>Add VAT to the invoice</t>
+  </si>
+  <si>
+    <t>Change the price of destination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropdown box of users </t>
   </si>
 </sst>
 </file>
@@ -716,13 +749,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -739,6 +765,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2192,9 +2225,39 @@
             <c:strRef>
               <c:f>'Sprint 3'!$C$12:$C$28</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Create the Google Map Servlet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test Cases (1-5)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test Cases (6-10)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adding reporting functionality</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Refactoring code</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Refactoring code</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Display customer served per day</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Create a daily report</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Add VAT to the invoice</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Change the price of destination</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dropdown box of users </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2207,6 +2270,36 @@
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>43435</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43437</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43437</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43436</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2245,9 +2338,39 @@
             <c:strRef>
               <c:f>'Sprint 3'!$C$12:$C$28</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Create the Google Map Servlet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test Cases (1-5)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test Cases (6-10)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Adding reporting functionality</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Refactoring code</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Refactoring code</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Display customer served per day</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Create a daily report</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Add VAT to the invoice</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Change the price of destination</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dropdown box of users </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2259,6 +2382,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -4220,7 +4373,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table352" displayName="Table352" ref="B11:L28" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table352" displayName="Table352" ref="B11:L28" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="B11:L28"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID:" dataDxfId="10"/>
@@ -5096,7 +5249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
@@ -5717,8 +5870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5729,6 +5882,8 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
@@ -5876,132 +6031,296 @@
       <c r="L12" s="15"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="19">
+        <v>43437</v>
+      </c>
+      <c r="G13" s="19">
+        <v>43438</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J13" s="20"/>
       <c r="K13" s="25"/>
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="B14" s="10">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
+      </c>
+      <c r="F14" s="19">
+        <v>43437</v>
+      </c>
+      <c r="G14" s="19">
+        <v>43438</v>
+      </c>
+      <c r="H14" s="9">
+        <v>2</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J14" s="20"/>
       <c r="K14" s="25"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>4</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="19">
+        <v>43436</v>
+      </c>
+      <c r="G15" s="31">
+        <v>43437</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J15" s="20"/>
       <c r="K15" s="25"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="B16" s="10">
+        <v>5</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="19">
+        <v>43436</v>
+      </c>
+      <c r="G16" s="31">
+        <v>43437</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J16" s="20"/>
       <c r="K16" s="25"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="B17" s="10">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="19">
+        <v>43436</v>
+      </c>
+      <c r="G17" s="19">
+        <v>43437</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J17" s="20"/>
       <c r="K17" s="25"/>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
+    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>7</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="19">
+        <v>43437</v>
+      </c>
+      <c r="G18" s="19">
+        <v>43438</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J18" s="20"/>
       <c r="K18" s="25"/>
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="20"/>
+      <c r="B19" s="10">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="19">
+        <v>43436</v>
+      </c>
+      <c r="G19" s="19">
+        <v>43437</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="20">
+        <v>1</v>
+      </c>
       <c r="K19" s="25"/>
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="B20" s="10">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="19">
+        <v>43437</v>
+      </c>
+      <c r="G20" s="19">
+        <v>43438</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J20" s="20"/>
       <c r="K20" s="25"/>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="20"/>
+    <row r="21" spans="2:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10">
+        <v>10</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="19">
+        <v>43436</v>
+      </c>
+      <c r="G21" s="19">
+        <v>43436</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="20">
+        <v>1</v>
+      </c>
       <c r="K21" s="25"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="30"/>
+    <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1</v>
+      </c>
+      <c r="F22" s="28">
+        <v>43436</v>
+      </c>
+      <c r="G22" s="29">
+        <v>43436</v>
+      </c>
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="30">
+        <v>1</v>
+      </c>
       <c r="K22" s="26"/>
       <c r="L22" s="9"/>
     </row>

</xml_diff>